<commit_message>
Updates to Performer (looping through reports, storing files, etc.)
</commit_message>
<xml_diff>
--- a/GenerateYearlyReportPerformer/Data/Config.xlsx
+++ b/GenerateYearlyReportPerformer/Data/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Name</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Credentials for ACME System 1</t>
   </si>
   <si>
-    <t>DownloadReportsFolderPath</t>
-  </si>
-  <si>
     <t>Data\Temp</t>
   </si>
   <si>
@@ -145,6 +142,12 @@
   </si>
   <si>
     <t>Year, for which reporst should be generated</t>
+  </si>
+  <si>
+    <t>ReportsDownloadPath</t>
+  </si>
+  <si>
+    <t>Place to download monthly reports</t>
   </si>
 </sst>
 </file>
@@ -516,7 +519,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -526,7 +529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -621,13 +624,13 @@
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" s="6">
         <v>2020</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1629,8 +1632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1700,10 +1703,13 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>39</v>
+      <c r="C5" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Adding generation of yearly report.
</commit_message>
<xml_diff>
--- a/GenerateYearlyReportPerformer/Data/Config.xlsx
+++ b/GenerateYearlyReportPerformer/Data/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -519,7 +519,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -529,7 +529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1632,8 +1632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>